<commit_message>
Update RQ1 cortex outputs, metric concordance tables, p-value datasets, and refine analysis scripts
</commit_message>
<xml_diff>
--- a/data/raw/PSY_adults.xlsx
+++ b/data/raw/PSY_adults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\Git_META\META\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE17D74-B710-409B-9713-2D1341E02982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7694332B-FD43-405B-AB5A-9279242A2BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="2115" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -652,8 +652,8 @@
   </sheetPr>
   <dimension ref="A1:X1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>